<commit_message>
updated audiogram to work for group-data
</commit_message>
<xml_diff>
--- a/aud_data.xlsx
+++ b/aud_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Desktop\psychoacoustic_course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1113A4EA-A56F-43EF-87D1-8A44B675DB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2E8CC9-45AD-4D15-AF88-6DC04616035A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9015" yWindow="3420" windowWidth="22650" windowHeight="15015" xr2:uid="{C162A1AB-BBAC-4080-8EF6-98ADD63A2EC9}"/>
+    <workbookView xWindow="4050" yWindow="3825" windowWidth="22650" windowHeight="15015" xr2:uid="{C162A1AB-BBAC-4080-8EF6-98ADD63A2EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>L125</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -450,71 +453,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E9C065-EFAD-4D68-846E-5E47D2F1A7FD}">
-  <dimension ref="A1:AK9"/>
+  <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -532,477 +539,502 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>9</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>-3</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-5</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>18</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>-5</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>-4</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>15</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>16</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>-5</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>15</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>18</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>-4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>19</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>22</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>16</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>24</v>
-      </c>
-      <c r="K3">
-        <v>11</v>
       </c>
       <c r="L3">
         <v>11</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
         <v>16</v>
       </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
       <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
         <v>19</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>-3</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>12</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>18</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>17</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>13</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
       <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
         <v>15</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>17</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>22</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>13</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>23</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>8</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>22</v>
       </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
       <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>17</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>-4</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>25</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>-3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>-1</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>25</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>10</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>6</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>13</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>14</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>-5</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>20</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>-3</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>15</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-1</v>
       </c>
-      <c r="D6">
-        <f>D15+B12</f>
+      <c r="E6">
+        <f>E15+C12</f>
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>-3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>13</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>21</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>11</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>22</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>12</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>15</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>8</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>-1</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>24</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>-4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>20</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>17</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>25</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>-3</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>14</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>20</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>-2</v>
-      </c>
-      <c r="P7">
-        <v>7</v>
       </c>
       <c r="Q7">
         <v>7</v>
       </c>
       <c r="R7">
+        <v>7</v>
+      </c>
+      <c r="S7">
         <v>10</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
       <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>-4</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>16</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>14</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>6</v>
       </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
       <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
         <v>6</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>15</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>16</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>4</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>12</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>-5</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>-2</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>16</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
       <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
         <v>-1</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>22</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>24</v>
-      </c>
-      <c r="L9">
-        <v>9</v>
       </c>
       <c r="M9">
         <v>9</v>
       </c>
       <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9">
         <v>0</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>24</v>
-      </c>
-      <c r="P9">
-        <v>5</v>
       </c>
       <c r="Q9">
         <v>5</v>
       </c>
       <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
         <v>16</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>15</v>
       </c>
     </row>

</xml_diff>